<commit_message>
ETF NAV RTD from 체크 터미널
</commit_message>
<xml_diff>
--- a/RealTimeData_Visualization/ETF NAV 실시간 데이터 Check.xlsx
+++ b/RealTimeData_Visualization/ETF NAV 실시간 데이터 Check.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\check\desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Check\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD638AF-6376-44F5-841A-77BAEE775CD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71A9CEC-8167-47E4-98B0-82F5128DAAA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" xr2:uid="{DD9532F0-B415-4463-A875-8AD824D9D717}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>NAV</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +36,50 @@
   </si>
   <si>
     <t>차이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종목명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KODEX 200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종목코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>069500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거래량</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iNAV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ETF-iNAV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>괴리율 (%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지수기준가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAV-지수기준가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -45,7 +89,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="190" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -97,11 +141,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -127,25 +177,55 @@
   <volType type="realTimeData">
     <main first="checkexpert.rtd">
       <tp>
-        <v>39388.36</v>
+        <v>39425.17</v>
         <stp/>
         <stp>15301</stp>
         <stp>069500</stp>
         <tr r="A1" s="1"/>
+        <tr r="G9" s="1"/>
       </tp>
       <tp>
-        <v>-53.36</v>
+        <v>-15.17</v>
         <stp/>
         <stp>15305</stp>
         <stp>069500</stp>
         <tr r="A4" s="1"/>
       </tp>
       <tp>
-        <v>39335</v>
+        <v>-0.03</v>
+        <stp/>
+        <stp>15304</stp>
+        <stp>069500</stp>
+        <tr r="H11" s="1"/>
+      </tp>
+      <tp>
+        <v>39410</v>
         <stp/>
         <stp>15001</stp>
         <stp>069500</stp>
         <tr r="A2" s="1"/>
+        <tr r="G7" s="1"/>
+      </tp>
+      <tp>
+        <v>39310</v>
+        <stp/>
+        <stp>33405</stp>
+        <stp>069500</stp>
+        <tr r="G12" s="1"/>
+      </tp>
+      <tp>
+        <v>115.17</v>
+        <stp/>
+        <stp>33406</stp>
+        <stp>069500</stp>
+        <tr r="H13" s="1"/>
+      </tp>
+      <tp>
+        <v>1564839</v>
+        <stp/>
+        <stp>30620</stp>
+        <stp>069500</stp>
+        <tr r="G8" s="1"/>
       </tp>
     </main>
   </volType>
@@ -449,51 +529,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8EC754-C12A-4D4B-B432-3FDA3A33A400}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <f>RTD("checkexpert.rtd",,"15301","069500")</f>
-        <v>39388.36</v>
+        <v>39425.17</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f>RTD("checkexpert.rtd",,"15001","069500")</f>
-        <v>39335</v>
+        <v>39410</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>A2-A1</f>
-        <v>-53.360000000000582</v>
+        <v>-15.169999999998254</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>RTD("checkexpert.rtd",,"15305","069500")</f>
-        <v>-53.36</v>
+        <v>-15.17</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
+        <f>RTD("checkexpert.rtd",,"15001",G5)</f>
+        <v>39410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1">
+        <f>RTD("checkexpert.rtd",,"30620",G5)</f>
+        <v>1564839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1">
+        <f>RTD("checkexpert.rtd",,"15301",G5)</f>
+        <v>39425.17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1">
+        <f>G7-G9</f>
+        <v>-15.169999999998254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="1">
+        <f>(G10)/G9*100</f>
+        <v>-3.8477957102019483E-2</v>
+      </c>
+      <c r="H11" s="3">
+        <f>RTD("checkexpert.rtd",,"15304",G5)</f>
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="1">
+        <f>RTD("checkexpert.rtd",,"33405",G5)</f>
+        <v>39310</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="1">
+        <f>G9-G12</f>
+        <v>115.16999999999825</v>
+      </c>
+      <c r="H13" s="3">
+        <f>RTD("checkexpert.rtd",,"33406",G5)</f>
+        <v>115.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>